<commit_message>
Fixed callouts and removed Excel save
</commit_message>
<xml_diff>
--- a/SearchTerms.xlsx
+++ b/SearchTerms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefan.reutter\Documents\UiPath\SharedDemos\WikipediaRevenues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC04B057-B27C-48D4-935A-1C8FC19DD786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA8B699-5121-4BB3-B59E-5D1F64B7FF12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2567" yWindow="2567" windowWidth="19200" windowHeight="10073" xr2:uid="{F99B54F5-476C-4F3C-B1A4-06AF5F1D984B}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{F99B54F5-476C-4F3C-B1A4-06AF5F1D984B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>